<commit_message>
forgot to add a tonne of stuff
</commit_message>
<xml_diff>
--- a/test data/IBSC Student Scots 7TGAR1.xlsx
+++ b/test data/IBSC Student Scots 7TGAR1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3c85ca06803d405f/2017-2019/Documents/RF/IBSC Survey Feedback/Master Dash/test data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BCD307A3-17FC-49D8-8361-AA8CF4712A75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="8_{BCD307A3-17FC-49D8-8361-AA8CF4712A75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C2FE875C-9280-4CF7-88AF-71B1C8474FCA}"/>
   <bookViews>
-    <workbookView xWindow="44170" yWindow="1520" windowWidth="28450" windowHeight="19350" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="39770" yWindow="2350" windowWidth="28450" windowHeight="17110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Node Attributes" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,6 @@
     <sheet name="Relationship Question 4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -753,11 +752,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AI12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.58203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.58203125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="20.75" customWidth="1"/>
+    <col min="30" max="30" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="12.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -864,7 +874,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -971,7 +981,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>56</v>
       </c>
@@ -1078,7 +1088,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>64</v>
       </c>
@@ -1185,7 +1195,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>69</v>
       </c>
@@ -1292,7 +1302,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>76</v>
       </c>
@@ -1399,7 +1409,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>82</v>
       </c>
@@ -1506,7 +1516,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>86</v>
       </c>
@@ -1613,7 +1623,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>91</v>
       </c>
@@ -1720,7 +1730,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>95</v>
       </c>
@@ -1827,7 +1837,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>99</v>
       </c>
@@ -1934,7 +1944,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>104</v>
       </c>
@@ -2044,7 +2054,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:AI12" numberStoredAsText="1"/>
+    <ignoredError sqref="A2:AI12 B1:AI1" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -2053,11 +2063,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D121"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A16" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>111</v>
       </c>
@@ -2071,7 +2081,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -2085,7 +2095,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>35</v>
       </c>
@@ -2099,7 +2109,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>35</v>
       </c>
@@ -2113,7 +2123,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>35</v>
       </c>
@@ -2127,7 +2137,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>35</v>
       </c>
@@ -2141,7 +2151,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -2155,7 +2165,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>35</v>
       </c>
@@ -2169,7 +2179,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>35</v>
       </c>
@@ -2183,7 +2193,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>35</v>
       </c>
@@ -2197,7 +2207,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>35</v>
       </c>
@@ -2211,7 +2221,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>35</v>
       </c>
@@ -2225,7 +2235,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>56</v>
       </c>
@@ -2239,7 +2249,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>56</v>
       </c>
@@ -2253,7 +2263,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>56</v>
       </c>
@@ -2267,7 +2277,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>56</v>
       </c>
@@ -2281,7 +2291,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>56</v>
       </c>
@@ -2295,7 +2305,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>56</v>
       </c>
@@ -2309,7 +2319,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>56</v>
       </c>
@@ -2323,7 +2333,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>56</v>
       </c>
@@ -2337,7 +2347,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>56</v>
       </c>
@@ -2351,7 +2361,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>56</v>
       </c>
@@ -2365,7 +2375,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>56</v>
       </c>
@@ -2379,7 +2389,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>64</v>
       </c>
@@ -2393,7 +2403,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>64</v>
       </c>
@@ -2407,7 +2417,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>64</v>
       </c>
@@ -2421,7 +2431,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>64</v>
       </c>
@@ -2435,7 +2445,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>64</v>
       </c>
@@ -2449,7 +2459,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>64</v>
       </c>
@@ -2463,7 +2473,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>64</v>
       </c>
@@ -2477,7 +2487,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>64</v>
       </c>
@@ -2491,7 +2501,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>64</v>
       </c>
@@ -2505,7 +2515,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>64</v>
       </c>
@@ -2519,7 +2529,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>64</v>
       </c>
@@ -2533,7 +2543,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>69</v>
       </c>
@@ -2547,7 +2557,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>69</v>
       </c>
@@ -2561,7 +2571,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>69</v>
       </c>
@@ -2575,7 +2585,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>69</v>
       </c>
@@ -2589,7 +2599,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>69</v>
       </c>
@@ -2603,7 +2613,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>69</v>
       </c>
@@ -2617,7 +2627,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>69</v>
       </c>
@@ -2631,7 +2641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>69</v>
       </c>
@@ -2645,7 +2655,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>69</v>
       </c>
@@ -2659,7 +2669,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>69</v>
       </c>
@@ -2673,7 +2683,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>69</v>
       </c>
@@ -2687,7 +2697,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>76</v>
       </c>
@@ -2701,7 +2711,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>76</v>
       </c>
@@ -2715,7 +2725,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>76</v>
       </c>
@@ -2729,7 +2739,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>76</v>
       </c>
@@ -2743,7 +2753,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>76</v>
       </c>
@@ -2757,7 +2767,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>76</v>
       </c>
@@ -2771,7 +2781,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>76</v>
       </c>
@@ -2785,7 +2795,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>76</v>
       </c>
@@ -2799,7 +2809,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>76</v>
       </c>
@@ -2813,7 +2823,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>76</v>
       </c>
@@ -2827,7 +2837,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>76</v>
       </c>
@@ -2841,7 +2851,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>82</v>
       </c>
@@ -2855,7 +2865,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>82</v>
       </c>
@@ -2869,7 +2879,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>82</v>
       </c>
@@ -2883,7 +2893,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>82</v>
       </c>
@@ -2897,7 +2907,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>82</v>
       </c>
@@ -2911,7 +2921,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>82</v>
       </c>
@@ -2925,7 +2935,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>82</v>
       </c>
@@ -2939,7 +2949,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>82</v>
       </c>
@@ -2953,7 +2963,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>82</v>
       </c>
@@ -2967,7 +2977,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>82</v>
       </c>
@@ -2981,7 +2991,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>86</v>
       </c>
@@ -2995,7 +3005,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>86</v>
       </c>
@@ -3009,7 +3019,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>86</v>
       </c>
@@ -3023,7 +3033,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>86</v>
       </c>
@@ -3037,7 +3047,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>86</v>
       </c>
@@ -3051,7 +3061,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>86</v>
       </c>
@@ -3065,7 +3075,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>86</v>
       </c>
@@ -3079,7 +3089,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>86</v>
       </c>
@@ -3093,7 +3103,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>86</v>
       </c>
@@ -3107,7 +3117,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>86</v>
       </c>
@@ -3121,7 +3131,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>86</v>
       </c>
@@ -3135,7 +3145,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>91</v>
       </c>
@@ -3149,7 +3159,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>91</v>
       </c>
@@ -3163,7 +3173,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>91</v>
       </c>
@@ -3177,7 +3187,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>91</v>
       </c>
@@ -3191,7 +3201,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>91</v>
       </c>
@@ -3205,7 +3215,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>91</v>
       </c>
@@ -3219,7 +3229,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>91</v>
       </c>
@@ -3233,7 +3243,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>91</v>
       </c>
@@ -3247,7 +3257,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>91</v>
       </c>
@@ -3261,7 +3271,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>91</v>
       </c>
@@ -3275,7 +3285,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>91</v>
       </c>
@@ -3289,7 +3299,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>95</v>
       </c>
@@ -3303,7 +3313,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>95</v>
       </c>
@@ -3317,7 +3327,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>95</v>
       </c>
@@ -3331,7 +3341,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>95</v>
       </c>
@@ -3345,7 +3355,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>95</v>
       </c>
@@ -3359,7 +3369,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>95</v>
       </c>
@@ -3373,7 +3383,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>95</v>
       </c>
@@ -3387,7 +3397,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>95</v>
       </c>
@@ -3401,7 +3411,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>95</v>
       </c>
@@ -3415,7 +3425,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>95</v>
       </c>
@@ -3429,7 +3439,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>95</v>
       </c>
@@ -3443,7 +3453,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>99</v>
       </c>
@@ -3457,7 +3467,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>99</v>
       </c>
@@ -3471,7 +3481,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>99</v>
       </c>
@@ -3485,7 +3495,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>99</v>
       </c>
@@ -3499,7 +3509,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>99</v>
       </c>
@@ -3513,7 +3523,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>99</v>
       </c>
@@ -3527,7 +3537,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>99</v>
       </c>
@@ -3541,7 +3551,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>99</v>
       </c>
@@ -3555,7 +3565,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>99</v>
       </c>
@@ -3569,7 +3579,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>99</v>
       </c>
@@ -3583,7 +3593,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>99</v>
       </c>
@@ -3597,7 +3607,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>104</v>
       </c>
@@ -3611,7 +3621,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>104</v>
       </c>
@@ -3625,7 +3635,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>104</v>
       </c>
@@ -3639,7 +3649,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>104</v>
       </c>
@@ -3653,7 +3663,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>104</v>
       </c>
@@ -3667,7 +3677,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>104</v>
       </c>
@@ -3681,7 +3691,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>104</v>
       </c>
@@ -3695,7 +3705,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>104</v>
       </c>
@@ -3709,7 +3719,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>104</v>
       </c>
@@ -3723,7 +3733,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>104</v>
       </c>
@@ -3737,7 +3747,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>104</v>
       </c>
@@ -3765,9 +3775,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>111</v>
       </c>
@@ -3781,7 +3791,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -3795,7 +3805,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>35</v>
       </c>
@@ -3809,7 +3819,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>35</v>
       </c>
@@ -3823,7 +3833,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>35</v>
       </c>
@@ -3837,7 +3847,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>35</v>
       </c>
@@ -3851,7 +3861,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -3865,7 +3875,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>35</v>
       </c>
@@ -3879,7 +3889,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>35</v>
       </c>
@@ -3893,7 +3903,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>35</v>
       </c>
@@ -3907,7 +3917,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>35</v>
       </c>
@@ -3921,7 +3931,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>35</v>
       </c>
@@ -3935,7 +3945,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>56</v>
       </c>
@@ -3949,7 +3959,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>56</v>
       </c>
@@ -3963,7 +3973,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>56</v>
       </c>
@@ -3977,7 +3987,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>56</v>
       </c>
@@ -3991,7 +4001,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>56</v>
       </c>
@@ -4005,7 +4015,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>56</v>
       </c>
@@ -4019,7 +4029,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>56</v>
       </c>
@@ -4033,7 +4043,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>56</v>
       </c>
@@ -4047,7 +4057,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>56</v>
       </c>
@@ -4061,7 +4071,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>56</v>
       </c>
@@ -4075,7 +4085,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>56</v>
       </c>
@@ -4089,7 +4099,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>64</v>
       </c>
@@ -4103,7 +4113,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>64</v>
       </c>
@@ -4117,7 +4127,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>64</v>
       </c>
@@ -4131,7 +4141,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>64</v>
       </c>
@@ -4145,7 +4155,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>64</v>
       </c>
@@ -4159,7 +4169,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>64</v>
       </c>
@@ -4173,7 +4183,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>64</v>
       </c>
@@ -4187,7 +4197,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>64</v>
       </c>
@@ -4201,7 +4211,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>64</v>
       </c>
@@ -4215,7 +4225,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>64</v>
       </c>
@@ -4229,7 +4239,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>64</v>
       </c>
@@ -4243,7 +4253,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>69</v>
       </c>
@@ -4257,7 +4267,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>69</v>
       </c>
@@ -4271,7 +4281,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>69</v>
       </c>
@@ -4285,7 +4295,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>69</v>
       </c>
@@ -4299,7 +4309,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>69</v>
       </c>
@@ -4313,7 +4323,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>69</v>
       </c>
@@ -4327,7 +4337,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>69</v>
       </c>
@@ -4341,7 +4351,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>69</v>
       </c>
@@ -4355,7 +4365,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>69</v>
       </c>
@@ -4369,7 +4379,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>69</v>
       </c>
@@ -4383,7 +4393,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>69</v>
       </c>
@@ -4397,7 +4407,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>76</v>
       </c>
@@ -4411,7 +4421,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>76</v>
       </c>
@@ -4425,7 +4435,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>76</v>
       </c>
@@ -4439,7 +4449,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>76</v>
       </c>
@@ -4453,7 +4463,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>76</v>
       </c>
@@ -4467,7 +4477,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>76</v>
       </c>
@@ -4481,7 +4491,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>76</v>
       </c>
@@ -4495,7 +4505,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>76</v>
       </c>
@@ -4509,7 +4519,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>76</v>
       </c>
@@ -4523,7 +4533,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>76</v>
       </c>
@@ -4537,7 +4547,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>76</v>
       </c>
@@ -4551,7 +4561,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>82</v>
       </c>
@@ -4565,7 +4575,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>82</v>
       </c>
@@ -4579,7 +4589,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>82</v>
       </c>
@@ -4593,7 +4603,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>82</v>
       </c>
@@ -4607,7 +4617,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>82</v>
       </c>
@@ -4621,7 +4631,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>82</v>
       </c>
@@ -4635,7 +4645,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>82</v>
       </c>
@@ -4649,7 +4659,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>82</v>
       </c>
@@ -4663,7 +4673,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>82</v>
       </c>
@@ -4677,7 +4687,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>82</v>
       </c>
@@ -4691,7 +4701,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>86</v>
       </c>
@@ -4705,7 +4715,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>86</v>
       </c>
@@ -4719,7 +4729,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>86</v>
       </c>
@@ -4733,7 +4743,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>86</v>
       </c>
@@ -4747,7 +4757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>86</v>
       </c>
@@ -4761,7 +4771,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>86</v>
       </c>
@@ -4775,7 +4785,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>86</v>
       </c>
@@ -4789,7 +4799,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>86</v>
       </c>
@@ -4803,7 +4813,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>86</v>
       </c>
@@ -4817,7 +4827,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>86</v>
       </c>
@@ -4831,7 +4841,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>86</v>
       </c>
@@ -4845,7 +4855,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>91</v>
       </c>
@@ -4859,7 +4869,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>91</v>
       </c>
@@ -4873,7 +4883,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>91</v>
       </c>
@@ -4887,7 +4897,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>91</v>
       </c>
@@ -4901,7 +4911,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>91</v>
       </c>
@@ -4915,7 +4925,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>91</v>
       </c>
@@ -4929,7 +4939,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>91</v>
       </c>
@@ -4943,7 +4953,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>91</v>
       </c>
@@ -4957,7 +4967,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>91</v>
       </c>
@@ -4971,7 +4981,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>91</v>
       </c>
@@ -4985,7 +4995,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>91</v>
       </c>
@@ -4999,7 +5009,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>95</v>
       </c>
@@ -5013,7 +5023,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>95</v>
       </c>
@@ -5027,7 +5037,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>95</v>
       </c>
@@ -5041,7 +5051,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>95</v>
       </c>
@@ -5055,7 +5065,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>95</v>
       </c>
@@ -5069,7 +5079,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>95</v>
       </c>
@@ -5083,7 +5093,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>95</v>
       </c>
@@ -5097,7 +5107,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>95</v>
       </c>
@@ -5111,7 +5121,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>95</v>
       </c>
@@ -5125,7 +5135,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>95</v>
       </c>
@@ -5139,7 +5149,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>95</v>
       </c>
@@ -5153,7 +5163,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>99</v>
       </c>
@@ -5167,7 +5177,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>99</v>
       </c>
@@ -5181,7 +5191,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>99</v>
       </c>
@@ -5195,7 +5205,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>99</v>
       </c>
@@ -5209,7 +5219,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>99</v>
       </c>
@@ -5223,7 +5233,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>99</v>
       </c>
@@ -5237,7 +5247,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>99</v>
       </c>
@@ -5251,7 +5261,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>99</v>
       </c>
@@ -5265,7 +5275,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>99</v>
       </c>
@@ -5279,7 +5289,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>99</v>
       </c>
@@ -5293,7 +5303,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>99</v>
       </c>
@@ -5307,7 +5317,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>104</v>
       </c>
@@ -5321,7 +5331,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>104</v>
       </c>
@@ -5335,7 +5345,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>104</v>
       </c>
@@ -5349,7 +5359,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>104</v>
       </c>
@@ -5363,7 +5373,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>104</v>
       </c>
@@ -5377,7 +5387,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>104</v>
       </c>
@@ -5391,7 +5401,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>104</v>
       </c>
@@ -5405,7 +5415,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>104</v>
       </c>
@@ -5419,7 +5429,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>104</v>
       </c>
@@ -5433,7 +5443,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>104</v>
       </c>
@@ -5447,7 +5457,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>104</v>
       </c>
@@ -5475,9 +5485,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>111</v>
       </c>
@@ -5491,7 +5501,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -5505,7 +5515,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>35</v>
       </c>
@@ -5519,7 +5529,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>35</v>
       </c>
@@ -5533,7 +5543,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>35</v>
       </c>
@@ -5547,7 +5557,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>35</v>
       </c>
@@ -5561,7 +5571,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -5575,7 +5585,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>35</v>
       </c>
@@ -5589,7 +5599,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>35</v>
       </c>
@@ -5603,7 +5613,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>35</v>
       </c>
@@ -5617,7 +5627,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>35</v>
       </c>
@@ -5631,7 +5641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>35</v>
       </c>
@@ -5645,7 +5655,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>56</v>
       </c>
@@ -5659,7 +5669,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>56</v>
       </c>
@@ -5673,7 +5683,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>56</v>
       </c>
@@ -5687,7 +5697,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>56</v>
       </c>
@@ -5701,7 +5711,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>56</v>
       </c>
@@ -5715,7 +5725,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>56</v>
       </c>
@@ -5729,7 +5739,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>56</v>
       </c>
@@ -5743,7 +5753,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>56</v>
       </c>
@@ -5757,7 +5767,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>56</v>
       </c>
@@ -5771,7 +5781,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>56</v>
       </c>
@@ -5785,7 +5795,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>56</v>
       </c>
@@ -5799,7 +5809,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>64</v>
       </c>
@@ -5813,7 +5823,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>64</v>
       </c>
@@ -5827,7 +5837,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>64</v>
       </c>
@@ -5841,7 +5851,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>64</v>
       </c>
@@ -5855,7 +5865,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>64</v>
       </c>
@@ -5869,7 +5879,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>64</v>
       </c>
@@ -5883,7 +5893,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>64</v>
       </c>
@@ -5897,7 +5907,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>64</v>
       </c>
@@ -5911,7 +5921,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>64</v>
       </c>
@@ -5925,7 +5935,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>64</v>
       </c>
@@ -5939,7 +5949,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>64</v>
       </c>
@@ -5953,7 +5963,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>69</v>
       </c>
@@ -5967,7 +5977,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>69</v>
       </c>
@@ -5981,7 +5991,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>69</v>
       </c>
@@ -5995,7 +6005,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>69</v>
       </c>
@@ -6009,7 +6019,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>69</v>
       </c>
@@ -6023,7 +6033,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>69</v>
       </c>
@@ -6037,7 +6047,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>69</v>
       </c>
@@ -6051,7 +6061,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>69</v>
       </c>
@@ -6065,7 +6075,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>69</v>
       </c>
@@ -6079,7 +6089,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>69</v>
       </c>
@@ -6093,7 +6103,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>69</v>
       </c>
@@ -6107,7 +6117,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>76</v>
       </c>
@@ -6121,7 +6131,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>76</v>
       </c>
@@ -6135,7 +6145,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>76</v>
       </c>
@@ -6149,7 +6159,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>76</v>
       </c>
@@ -6163,7 +6173,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>76</v>
       </c>
@@ -6177,7 +6187,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>76</v>
       </c>
@@ -6191,7 +6201,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>76</v>
       </c>
@@ -6205,7 +6215,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>76</v>
       </c>
@@ -6219,7 +6229,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>76</v>
       </c>
@@ -6233,7 +6243,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>76</v>
       </c>
@@ -6247,7 +6257,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>76</v>
       </c>
@@ -6261,7 +6271,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>82</v>
       </c>
@@ -6275,7 +6285,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>82</v>
       </c>
@@ -6289,7 +6299,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>82</v>
       </c>
@@ -6303,7 +6313,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>82</v>
       </c>
@@ -6317,7 +6327,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>82</v>
       </c>
@@ -6331,7 +6341,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>82</v>
       </c>
@@ -6345,7 +6355,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>82</v>
       </c>
@@ -6359,7 +6369,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>82</v>
       </c>
@@ -6373,7 +6383,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>82</v>
       </c>
@@ -6387,7 +6397,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>82</v>
       </c>
@@ -6401,7 +6411,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>86</v>
       </c>
@@ -6415,7 +6425,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>86</v>
       </c>
@@ -6429,7 +6439,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>86</v>
       </c>
@@ -6443,7 +6453,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>86</v>
       </c>
@@ -6457,7 +6467,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>86</v>
       </c>
@@ -6471,7 +6481,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>86</v>
       </c>
@@ -6485,7 +6495,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>86</v>
       </c>
@@ -6499,7 +6509,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>86</v>
       </c>
@@ -6513,7 +6523,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>86</v>
       </c>
@@ -6527,7 +6537,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>86</v>
       </c>
@@ -6541,7 +6551,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>86</v>
       </c>
@@ -6555,7 +6565,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>91</v>
       </c>
@@ -6569,7 +6579,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>91</v>
       </c>
@@ -6583,7 +6593,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>91</v>
       </c>
@@ -6597,7 +6607,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>91</v>
       </c>
@@ -6611,7 +6621,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>91</v>
       </c>
@@ -6625,7 +6635,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>91</v>
       </c>
@@ -6639,7 +6649,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>91</v>
       </c>
@@ -6653,7 +6663,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>91</v>
       </c>
@@ -6667,7 +6677,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>91</v>
       </c>
@@ -6681,7 +6691,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>91</v>
       </c>
@@ -6695,7 +6705,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>95</v>
       </c>
@@ -6709,7 +6719,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>95</v>
       </c>
@@ -6723,7 +6733,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>95</v>
       </c>
@@ -6737,7 +6747,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>95</v>
       </c>
@@ -6751,7 +6761,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>95</v>
       </c>
@@ -6765,7 +6775,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>95</v>
       </c>
@@ -6779,7 +6789,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>95</v>
       </c>
@@ -6793,7 +6803,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>95</v>
       </c>
@@ -6807,7 +6817,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>95</v>
       </c>
@@ -6821,7 +6831,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>95</v>
       </c>
@@ -6835,7 +6845,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>95</v>
       </c>
@@ -6849,7 +6859,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>99</v>
       </c>
@@ -6863,7 +6873,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>99</v>
       </c>
@@ -6877,7 +6887,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>99</v>
       </c>
@@ -6891,7 +6901,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>99</v>
       </c>
@@ -6905,7 +6915,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>99</v>
       </c>
@@ -6919,7 +6929,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>99</v>
       </c>
@@ -6933,7 +6943,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>99</v>
       </c>
@@ -6947,7 +6957,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>99</v>
       </c>
@@ -6961,7 +6971,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>99</v>
       </c>
@@ -6975,7 +6985,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>99</v>
       </c>
@@ -6989,7 +6999,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>99</v>
       </c>
@@ -7003,7 +7013,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>104</v>
       </c>
@@ -7017,7 +7027,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>104</v>
       </c>
@@ -7031,7 +7041,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>104</v>
       </c>
@@ -7045,7 +7055,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>104</v>
       </c>
@@ -7059,7 +7069,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>104</v>
       </c>
@@ -7073,7 +7083,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>104</v>
       </c>
@@ -7087,7 +7097,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>104</v>
       </c>
@@ -7101,7 +7111,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>104</v>
       </c>
@@ -7115,7 +7125,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>104</v>
       </c>
@@ -7129,7 +7139,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>104</v>
       </c>
@@ -7143,7 +7153,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>104</v>
       </c>

</xml_diff>

<commit_message>
added looping for multiple class generation
</commit_message>
<xml_diff>
--- a/test data/IBSC Student Scots 7TGAR1.xlsx
+++ b/test data/IBSC Student Scots 7TGAR1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3c85ca06803d405f/2017-2019/Documents/RF/IBSC Survey Feedback/Master Dash/test data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="8_{BCD307A3-17FC-49D8-8361-AA8CF4712A75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C2FE875C-9280-4CF7-88AF-71B1C8474FCA}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="8_{BCD307A3-17FC-49D8-8361-AA8CF4712A75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{23FBC80E-68D1-403B-BFD5-5194DF0ADE8A}"/>
   <bookViews>
-    <workbookView xWindow="39770" yWindow="2350" windowWidth="28450" windowHeight="17110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38290" yWindow="-110" windowWidth="38620" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Node Attributes" sheetId="1" r:id="rId1"/>
@@ -752,8 +752,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AI12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -762,6 +762,11 @@
     <col min="4" max="4" width="12.58203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.25" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20.58203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.08203125" customWidth="1"/>
+    <col min="15" max="15" width="9" customWidth="1"/>
+    <col min="16" max="16" width="11.5" customWidth="1"/>
+    <col min="17" max="17" width="9.25" customWidth="1"/>
+    <col min="26" max="26" width="11.6640625" customWidth="1"/>
     <col min="27" max="27" width="20.75" customWidth="1"/>
     <col min="30" max="30" width="10.25" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="12.1640625" bestFit="1" customWidth="1"/>

</xml_diff>